<commit_message>
Code for Master Thesis
</commit_message>
<xml_diff>
--- a/Results.xlsx
+++ b/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pavli\Desktop\masterThesis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{60C0F268-1F0B-4379-BAE7-C5B8730AD2AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{789BF7C7-A9B9-4C74-AF9B-890C912E3486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12816" xr2:uid="{1FF9E3A9-6E4F-4DDF-B582-02AE754312EC}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t>Average Driver Satisfaction</t>
   </si>
@@ -57,6 +57,18 @@
   </si>
   <si>
     <t>Original customers, 30, each of them every day</t>
+  </si>
+  <si>
+    <t>All served everyday</t>
+  </si>
+  <si>
+    <t>Must-serve only</t>
+  </si>
+  <si>
+    <t>Additional customers, 45, randomly chose who is served</t>
+  </si>
+  <si>
+    <t>Not all served everyday, prob. 0.5</t>
   </si>
 </sst>
 </file>
@@ -428,14 +440,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{434F2F8D-CAE7-4183-8608-D9FFE03F4E46}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="N14" sqref="E9:N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="31.109375" customWidth="1"/>
     <col min="3" max="3" width="29.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -481,11 +494,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
       <c r="C2" t="s">
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0.75309999999999999</v>
+        <v>0.99909999999999999</v>
       </c>
       <c r="E2">
         <v>0.99239999999999995</v>
@@ -502,11 +518,32 @@
       <c r="I2">
         <v>0.99150000000000005</v>
       </c>
+      <c r="J2">
+        <v>0.99639999999999995</v>
+      </c>
+      <c r="K2">
+        <v>0.9859</v>
+      </c>
+      <c r="L2">
+        <v>0.98419999999999996</v>
+      </c>
+      <c r="M2">
+        <v>0.95120000000000005</v>
+      </c>
+      <c r="N2">
+        <v>0.84850000000000003</v>
+      </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
       <c r="C3" t="s">
         <v>1</v>
       </c>
+      <c r="D3">
+        <v>0.29799999999999999</v>
+      </c>
       <c r="E3">
         <v>0.34229999999999999</v>
       </c>
@@ -521,6 +558,21 @@
       </c>
       <c r="I3">
         <v>0.46870000000000001</v>
+      </c>
+      <c r="J3">
+        <v>0.66379999999999995</v>
+      </c>
+      <c r="K3">
+        <v>0.74519999999999997</v>
+      </c>
+      <c r="L3">
+        <v>0.81069999999999998</v>
+      </c>
+      <c r="M3">
+        <v>0.81489999999999996</v>
+      </c>
+      <c r="N3">
+        <v>0.81589999999999996</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.3">
@@ -545,6 +597,21 @@
       <c r="I4">
         <v>15</v>
       </c>
+      <c r="J4">
+        <v>10.25</v>
+      </c>
+      <c r="K4">
+        <v>8</v>
+      </c>
+      <c r="L4">
+        <v>6.25</v>
+      </c>
+      <c r="M4">
+        <v>2.25</v>
+      </c>
+      <c r="N4">
+        <v>0.75</v>
+      </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
@@ -568,6 +635,21 @@
       <c r="I5">
         <v>3</v>
       </c>
+      <c r="J5">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="K5">
+        <v>1.6</v>
+      </c>
+      <c r="L5">
+        <v>1.25</v>
+      </c>
+      <c r="M5">
+        <v>0.45</v>
+      </c>
+      <c r="N5">
+        <v>0.15</v>
+      </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
@@ -590,6 +672,243 @@
       </c>
       <c r="I6">
         <v>1.0301</v>
+      </c>
+      <c r="J6">
+        <v>0.96089999999999998</v>
+      </c>
+      <c r="K6">
+        <v>0.91339999999999999</v>
+      </c>
+      <c r="L6">
+        <v>0.89539999999999997</v>
+      </c>
+      <c r="M6">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="N6">
+        <v>0.81589999999999996</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0.1</v>
+      </c>
+      <c r="F9">
+        <v>0.2</v>
+      </c>
+      <c r="G9">
+        <v>0.3</v>
+      </c>
+      <c r="H9">
+        <v>0.4</v>
+      </c>
+      <c r="I9">
+        <v>0.5</v>
+      </c>
+      <c r="J9">
+        <v>0.6</v>
+      </c>
+      <c r="K9">
+        <v>0.7</v>
+      </c>
+      <c r="L9">
+        <v>0.8</v>
+      </c>
+      <c r="M9">
+        <v>0.9</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0.83779999999999999</v>
+      </c>
+      <c r="F10">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="G10">
+        <v>0.84199999999999997</v>
+      </c>
+      <c r="H10">
+        <v>0.82969999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.80120000000000002</v>
+      </c>
+      <c r="J10">
+        <v>0.79310000000000003</v>
+      </c>
+      <c r="K10">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="L10">
+        <v>0.78380000000000005</v>
+      </c>
+      <c r="M10">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="N10">
+        <v>0.78249999999999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0.48089999999999999</v>
+      </c>
+      <c r="F11">
+        <v>0.5161</v>
+      </c>
+      <c r="G11">
+        <v>0.67290000000000005</v>
+      </c>
+      <c r="H11">
+        <v>0.66469999999999996</v>
+      </c>
+      <c r="I11">
+        <v>0.66720000000000002</v>
+      </c>
+      <c r="J11">
+        <v>0.76049999999999995</v>
+      </c>
+      <c r="K11">
+        <v>0.76029999999999998</v>
+      </c>
+      <c r="L11">
+        <v>0.79479999999999995</v>
+      </c>
+      <c r="M11">
+        <v>0.80220000000000002</v>
+      </c>
+      <c r="N11">
+        <v>0.81010000000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>4.5</v>
+      </c>
+      <c r="G12">
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <v>3</v>
+      </c>
+      <c r="I12">
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <v>1.5</v>
+      </c>
+      <c r="K12">
+        <v>1.5</v>
+      </c>
+      <c r="L12">
+        <v>1.5</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C13" t="s">
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <v>0.8</v>
+      </c>
+      <c r="F13">
+        <v>0.9</v>
+      </c>
+      <c r="G13">
+        <v>0.6</v>
+      </c>
+      <c r="H13">
+        <v>0.6</v>
+      </c>
+      <c r="I13">
+        <v>0.6</v>
+      </c>
+      <c r="J13">
+        <v>0.3</v>
+      </c>
+      <c r="K13">
+        <v>0.3</v>
+      </c>
+      <c r="L13">
+        <v>0.3</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="E14">
+        <v>0.94610000000000005</v>
+      </c>
+      <c r="F14">
+        <v>0.90880000000000005</v>
+      </c>
+      <c r="G14">
+        <v>0.87529999999999997</v>
+      </c>
+      <c r="H14">
+        <v>0.8357</v>
+      </c>
+      <c r="I14">
+        <v>0.79420000000000002</v>
+      </c>
+      <c r="J14">
+        <v>0.79749999999999999</v>
+      </c>
+      <c r="K14">
+        <v>0.78769999999999996</v>
+      </c>
+      <c r="L14">
+        <v>0.80459999999999998</v>
+      </c>
+      <c r="M14">
+        <v>0.79959999999999998</v>
+      </c>
+      <c r="N14">
+        <v>0.81010000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>